<commit_message>
Versión ajustada a partir de las observaciones de la coordinadora
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion01/EsqueletoGuion_CS_07_01_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion01/EsqueletoGuion_CS_07_01_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="140" windowWidth="24160" windowHeight="14360" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="3400" yWindow="220" windowWidth="22000" windowHeight="13180" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="88">
   <si>
     <t>FICHA</t>
   </si>
@@ -1643,7 +1643,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2222,12 +2222,12 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F50" sqref="F50"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2235,8 +2235,9 @@
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="17.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="46.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="17.83203125" style="3" customWidth="1"/>
     <col min="8" max="8" width="64.1640625" customWidth="1"/>
     <col min="9" max="9" width="17.5" style="4" bestFit="1" customWidth="1"/>
   </cols>
@@ -2497,11 +2498,13 @@
       <c r="B14" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="7"/>
+      <c r="D14" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="7"/>
@@ -2515,9 +2518,7 @@
         <v>47</v>
       </c>
       <c r="C15" s="7"/>
-      <c r="D15" s="22" t="s">
-        <v>48</v>
-      </c>
+      <c r="D15" s="8"/>
       <c r="E15" s="8" t="s">
         <v>37</v>
       </c>
@@ -2534,7 +2535,9 @@
         <v>47</v>
       </c>
       <c r="C16" s="7"/>
-      <c r="D16" s="8"/>
+      <c r="D16" s="22" t="s">
+        <v>49</v>
+      </c>
       <c r="E16" s="8" t="s">
         <v>38</v>
       </c>
@@ -2551,8 +2554,8 @@
         <v>47</v>
       </c>
       <c r="C17" s="7"/>
-      <c r="D17" s="22" t="s">
-        <v>49</v>
+      <c r="D17" s="23" t="s">
+        <v>44</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>37</v>
@@ -2570,37 +2573,35 @@
         <v>47</v>
       </c>
       <c r="C18" s="7"/>
-      <c r="D18" s="23" t="s">
-        <v>44</v>
-      </c>
+      <c r="D18" s="24"/>
       <c r="E18" s="8" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
+      <c r="H18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="15" thickBot="1">
       <c r="A19" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="8" t="s">
-        <v>45</v>
-      </c>
+      <c r="B19" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
-      <c r="H19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
     </row>
     <row r="20" spans="1:9" ht="15" thickBot="1">
       <c r="A20" s="21" t="s">
@@ -2610,7 +2611,7 @@
         <v>51</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
@@ -2626,11 +2627,13 @@
       <c r="B21" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="7"/>
@@ -2644,14 +2647,14 @@
         <v>51</v>
       </c>
       <c r="C22" s="7"/>
-      <c r="D22" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
     </row>
@@ -2663,14 +2666,14 @@
         <v>51</v>
       </c>
       <c r="C23" s="7"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>37</v>
-      </c>
+      <c r="D23" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="24"/>
+      <c r="G23" s="8"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
     </row>
@@ -2682,13 +2685,11 @@
         <v>51</v>
       </c>
       <c r="C24" s="7"/>
-      <c r="D24" s="22" t="s">
-        <v>54</v>
-      </c>
+      <c r="D24" s="8"/>
       <c r="E24" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" s="24"/>
+        <v>38</v>
+      </c>
+      <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
@@ -2700,14 +2701,10 @@
       <c r="B25" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="7"/>
+      <c r="E25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25" s="2"/>
       <c r="I25" s="7"/>
     </row>
     <row r="26" spans="1:9" ht="15" thickBot="1">
@@ -2718,10 +2715,14 @@
         <v>51</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="7"/>
+        <v>41</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="15" thickBot="1">
       <c r="A27" s="21" t="s">
@@ -2734,7 +2735,7 @@
         <v>41</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I27" s="7" t="s">
         <v>35</v>
@@ -2747,15 +2748,14 @@
       <c r="B28" s="23" t="s">
         <v>51</v>
       </c>
+      <c r="D28" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="E28" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>35</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="H28" s="2"/>
+      <c r="I28" s="7"/>
     </row>
     <row r="29" spans="1:9" ht="15" thickBot="1">
       <c r="A29" s="21" t="s">
@@ -2764,10 +2764,10 @@
       <c r="B29" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="E29" s="3" t="s">
+      <c r="F29" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>37</v>
       </c>
       <c r="H29" s="2"/>
@@ -2780,11 +2780,8 @@
       <c r="B30" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="F30" s="22" t="s">
-        <v>56</v>
-      </c>
       <c r="G30" s="3" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="7"/>
@@ -2797,39 +2794,43 @@
         <v>51</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" spans="1:9" ht="15" thickBot="1">
+    <row r="32" spans="1:9" ht="29" thickBot="1">
       <c r="A32" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B32" s="23" t="s">
         <v>51</v>
       </c>
+      <c r="F32" s="25" t="s">
+        <v>58</v>
+      </c>
       <c r="G32" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="1:9" ht="29" thickBot="1">
+    <row r="33" spans="1:9" ht="15" thickBot="1">
       <c r="A33" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B33" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="F33" s="25" t="s">
-        <v>58</v>
-      </c>
       <c r="G33" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H33" s="2"/>
-      <c r="I33" s="7"/>
+        <v>41</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="34" spans="1:9" ht="15" thickBot="1">
       <c r="A34" s="21" t="s">
@@ -2839,14 +2840,10 @@
         <v>51</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>35</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="H34" s="2"/>
+      <c r="I34" s="7"/>
     </row>
     <row r="35" spans="1:9" ht="15" thickBot="1">
       <c r="A35" s="21" t="s">
@@ -2856,7 +2853,7 @@
         <v>51</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="7"/>
@@ -2869,36 +2866,36 @@
         <v>51</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="7"/>
     </row>
-    <row r="37" spans="1:9" ht="15" thickBot="1">
+    <row r="37" spans="1:9" ht="29" thickBot="1">
       <c r="A37" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B37" s="23" t="s">
         <v>51</v>
       </c>
+      <c r="F37" s="26" t="s">
+        <v>59</v>
+      </c>
       <c r="G37" s="3" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="7"/>
     </row>
-    <row r="38" spans="1:9" ht="29" thickBot="1">
+    <row r="38" spans="1:9" ht="15" thickBot="1">
       <c r="A38" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B38" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="F38" s="26" t="s">
-        <v>59</v>
-      </c>
       <c r="G38" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="7"/>
@@ -2910,8 +2907,11 @@
       <c r="B39" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="G39" s="3" t="s">
-        <v>40</v>
+      <c r="D39" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="7"/>
@@ -2923,31 +2923,28 @@
       <c r="B40" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D40" s="22" t="s">
-        <v>44</v>
-      </c>
       <c r="E40" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H40" s="2"/>
-      <c r="I40" s="7"/>
+        <v>45</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="41" spans="1:9" ht="15" thickBot="1">
       <c r="A41" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I41" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="B41" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H41" s="2"/>
+      <c r="I41" s="7"/>
     </row>
     <row r="42" spans="1:9" ht="15" thickBot="1">
       <c r="A42" s="21" t="s">
@@ -2957,7 +2954,7 @@
         <v>61</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="7"/>
@@ -2970,7 +2967,7 @@
         <v>61</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="7"/>
@@ -2983,7 +2980,7 @@
         <v>61</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="7"/>
@@ -2996,7 +2993,7 @@
         <v>61</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H45" s="2"/>
       <c r="I45" s="7"/>
@@ -3009,10 +3006,14 @@
         <v>61</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H46" s="2"/>
-      <c r="I46" s="7"/>
+        <v>45</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="47" spans="1:9" ht="15" thickBot="1">
       <c r="A47" s="21" t="s">
@@ -3022,14 +3023,10 @@
         <v>61</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="I47" s="7" t="s">
-        <v>35</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H47" s="2"/>
+      <c r="I47" s="7"/>
     </row>
     <row r="48" spans="1:9" ht="15" thickBot="1">
       <c r="A48" s="21" t="s">
@@ -3039,10 +3036,14 @@
         <v>61</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H48" s="2"/>
-      <c r="I48" s="7"/>
+        <v>41</v>
+      </c>
+      <c r="H48" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="49" spans="1:9" ht="15" thickBot="1">
       <c r="A49" s="21" t="s">
@@ -3051,15 +3052,14 @@
       <c r="B49" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H49" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="I49" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="D49" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H49" s="2"/>
+      <c r="I49" s="7"/>
     </row>
     <row r="50" spans="1:9" ht="15" thickBot="1">
       <c r="A50" s="21" t="s">
@@ -3068,31 +3068,31 @@
       <c r="B50" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D50" s="22" t="s">
-        <v>44</v>
-      </c>
       <c r="E50" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H50" s="2"/>
-      <c r="I50" s="7"/>
+        <v>45</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="51" spans="1:9" ht="15" thickBot="1">
       <c r="A51" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>61</v>
+        <v>64</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>65</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I51" s="7" t="s">
-        <v>35</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="H51" s="2"/>
+      <c r="I51" s="7"/>
     </row>
     <row r="52" spans="1:9" ht="15" thickBot="1">
       <c r="A52" s="21" t="s">
@@ -3101,10 +3101,10 @@
       <c r="B52" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="D52" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="E52" s="3" t="s">
+      <c r="F52" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="G52" s="3" t="s">
         <v>37</v>
       </c>
       <c r="H52" s="2"/>
@@ -3117,11 +3117,8 @@
       <c r="B53" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="F53" s="26" t="s">
-        <v>66</v>
-      </c>
       <c r="G53" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H53" s="2"/>
       <c r="I53" s="7"/>
@@ -3134,7 +3131,7 @@
         <v>64</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H54" s="2"/>
       <c r="I54" s="7"/>
@@ -3146,6 +3143,9 @@
       <c r="B55" s="22" t="s">
         <v>64</v>
       </c>
+      <c r="F55" s="22" t="s">
+        <v>67</v>
+      </c>
       <c r="G55" s="3" t="s">
         <v>37</v>
       </c>
@@ -3159,11 +3159,8 @@
       <c r="B56" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="F56" s="22" t="s">
-        <v>67</v>
-      </c>
       <c r="G56" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H56" s="2"/>
       <c r="I56" s="7"/>
@@ -3176,7 +3173,7 @@
         <v>64</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H57" s="2"/>
       <c r="I57" s="7"/>
@@ -3188,7 +3185,10 @@
       <c r="B58" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="G58" s="3" t="s">
+      <c r="D58" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E58" s="3" t="s">
         <v>37</v>
       </c>
       <c r="H58" s="2"/>
@@ -3201,10 +3201,10 @@
       <c r="B59" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="D59" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="E59" s="3" t="s">
+      <c r="F59" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="G59" s="3" t="s">
         <v>37</v>
       </c>
       <c r="H59" s="2"/>
@@ -3217,11 +3217,9 @@
       <c r="B60" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="F60" s="23" t="s">
-        <v>69</v>
-      </c>
+      <c r="F60" s="24"/>
       <c r="G60" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H60" s="2"/>
       <c r="I60" s="7"/>
@@ -3233,38 +3231,37 @@
       <c r="B61" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="F61" s="24"/>
       <c r="G61" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H61" s="2"/>
       <c r="I61" s="7"/>
     </row>
-    <row r="62" spans="1:9" ht="15" thickBot="1">
+    <row r="62" spans="1:9" ht="29" thickBot="1">
       <c r="A62" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B62" s="22" t="s">
         <v>64</v>
       </c>
+      <c r="F62" s="26" t="s">
+        <v>70</v>
+      </c>
       <c r="G62" s="3" t="s">
         <v>37</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="7"/>
     </row>
-    <row r="63" spans="1:9" ht="29" thickBot="1">
+    <row r="63" spans="1:9" ht="15" thickBot="1">
       <c r="A63" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B63" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="F63" s="26" t="s">
-        <v>70</v>
-      </c>
       <c r="G63" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H63" s="2"/>
       <c r="I63" s="7"/>
@@ -3277,7 +3274,7 @@
         <v>64</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H64" s="2"/>
       <c r="I64" s="7"/>
@@ -3289,43 +3286,47 @@
       <c r="B65" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="G65" s="3" t="s">
+      <c r="D65" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E65" s="3" t="s">
         <v>37</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="7"/>
     </row>
-    <row r="66" spans="1:9" ht="15" thickBot="1">
+    <row r="66" spans="1:9" ht="29" thickBot="1">
       <c r="A66" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B66" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="D66" s="22" t="s">
-        <v>71</v>
-      </c>
       <c r="E66" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H66" s="2"/>
-      <c r="I66" s="7"/>
-    </row>
-    <row r="67" spans="1:9" ht="29" thickBot="1">
+        <v>45</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I66" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="15" thickBot="1">
       <c r="A67" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B67" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H67" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="I67" s="7" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="15" thickBot="1">
@@ -3336,29 +3337,12 @@
         <v>74</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I68" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" ht="15" thickBot="1">
-      <c r="A69" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B69" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="C69" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H69" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I69" s="7"/>
+      <c r="I68" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
CS0701 y CS0802: SegDigital y Esqueletos cargados ok
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion01/EsqueletoGuion_CS_07_01_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion01/EsqueletoGuion_CS_07_01_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MCMarquez\Desktop\Versiones\CienciasSociales\fuentes\contenidos\grado07\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\CienciasSociales\fuentes\contenidos\grado07\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="225" windowWidth="22005" windowHeight="13185" tabRatio="729" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="3408" yWindow="226" windowWidth="22007" windowHeight="13186" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="83">
   <si>
     <t>FICHA</t>
   </si>
@@ -171,9 +171,6 @@
     <t>Practica</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: la caída del Imperio Romano de Occidente</t>
-  </si>
-  <si>
     <t>El Imperio Bizantino</t>
   </si>
   <si>
@@ -183,9 +180,6 @@
     <t>El Cisma de Oriente</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: el Imperio Bizantino</t>
-  </si>
-  <si>
     <t>El Imperio Islámico</t>
   </si>
   <si>
@@ -210,18 +204,9 @@
     <t>El Califato abasí o Califato de Bagdad</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: la expansión islámica</t>
-  </si>
-  <si>
     <t>El Imperio Carolingio</t>
   </si>
   <si>
-    <t>Comprende qué fue el Imperio Carolingio</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: el Imperio Carolingio</t>
-  </si>
-  <si>
     <t>El mundo afroasiático durante la Edad Media</t>
   </si>
   <si>
@@ -258,13 +243,7 @@
     <t>Evaluación</t>
   </si>
   <si>
-    <t>Nuevos reinos</t>
-  </si>
-  <si>
     <t>Comprender cómo el fin de una época (el Imperio Romano) es el comienzo de otra nueva con otros protagonistas y circunstancias (Imperio Bizantino, mundo musulmán, Imperio de Carlomagno).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Refuerza importancia histórica de los imperios afroasiáticos en el medioevo europeo tu aprendizaje: </t>
   </si>
   <si>
     <t>Mapa conceptual</t>
@@ -303,9 +282,6 @@
     </r>
   </si>
   <si>
-    <t>Textoo</t>
-  </si>
-  <si>
     <t>El Califato Ortodoxo</t>
   </si>
   <si>
@@ -316,12 +292,6 @@
   </si>
   <si>
     <t>Conoce el Imperio bizantino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Refuerza tu aprendizaje: Importancia histórica de los imperios afroasiáticos </t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: Conoce el Imperio Bizantino</t>
   </si>
 </sst>
 </file>
@@ -1677,13 +1647,13 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="104.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="2" max="2" width="104.265625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>8</v>
       </c>
@@ -1691,7 +1661,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
@@ -1699,23 +1669,23 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="10" t="s">
         <v>1</v>
       </c>
@@ -1723,7 +1693,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="10" t="s">
         <v>12</v>
       </c>
@@ -1746,26 +1716,26 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.86328125" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="2"/>
-    <col min="2" max="2" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.86328125" style="2"/>
+    <col min="2" max="2" width="9.265625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="2"/>
-    <col min="9" max="10" width="15.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.85546875" style="2"/>
+    <col min="4" max="4" width="51.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.73046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.86328125" style="2"/>
+    <col min="9" max="10" width="15.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.73046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.86328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -1785,7 +1755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -1805,7 +1775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -1825,27 +1795,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" t="s">
         <v>82</v>
       </c>
-      <c r="D4" t="s">
-        <v>90</v>
-      </c>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1865,7 +1835,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1885,7 +1855,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -1905,7 +1875,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1916,7 +1886,7 @@
         <v>28</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>30</v>
@@ -1925,7 +1895,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -1945,27 +1915,27 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F10" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1999,18 +1969,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.86328125" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="66.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.85546875" style="2"/>
+    <col min="1" max="1" width="66.1328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.86328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
         <v>3</v>
       </c>
@@ -2021,40 +1991,40 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="17" customFormat="1" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C2" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C3" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C4" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2079,19 +2049,19 @@
   </sheetPr>
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.73046875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="19" t="s">
         <v>5</v>
       </c>
@@ -2102,7 +2072,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2113,7 +2083,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2124,18 +2094,18 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>92</v>
+      <c r="B4" t="s">
+        <v>82</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2146,7 +2116,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2157,7 +2127,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2168,84 +2138,84 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>80</v>
+      <c r="B8" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>83</v>
+      <c r="B10" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C27" s="5"/>
     </row>
   </sheetData>
@@ -2266,25 +2236,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView zoomScale="61" zoomScaleNormal="61" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="61" zoomScaleNormal="61" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
+      <selection pane="bottomLeft" activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="46.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="17.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="64.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.73046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="46.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="17.86328125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="64.1328125" customWidth="1"/>
+    <col min="9" max="9" width="17.3984375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="19" t="s">
         <v>6</v>
       </c>
@@ -2313,7 +2283,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="21" t="s">
         <v>19</v>
       </c>
@@ -2330,7 +2300,7 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="21" t="s">
         <v>19</v>
       </c>
@@ -2347,7 +2317,7 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="21" t="s">
         <v>19</v>
       </c>
@@ -2365,7 +2335,7 @@
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="21" t="s">
         <v>19</v>
       </c>
@@ -2383,7 +2353,7 @@
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="21" t="s">
         <v>19</v>
       </c>
@@ -2406,7 +2376,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="21" t="s">
         <v>19</v>
       </c>
@@ -2417,7 +2387,7 @@
         <v>38</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>37</v>
@@ -2427,7 +2397,7 @@
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="21" t="s">
         <v>19</v>
       </c>
@@ -2436,7 +2406,7 @@
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="23" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="22" t="s">
@@ -2448,7 +2418,7 @@
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="21" t="s">
         <v>19</v>
       </c>
@@ -2457,7 +2427,7 @@
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="23" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="22" t="s">
@@ -2469,7 +2439,7 @@
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="21" t="s">
         <v>19</v>
       </c>
@@ -2478,7 +2448,7 @@
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="23" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="22" t="s">
@@ -2490,7 +2460,7 @@
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="21" t="s">
         <v>19</v>
       </c>
@@ -2508,7 +2478,7 @@
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="21" t="s">
         <v>19</v>
       </c>
@@ -2524,18 +2494,18 @@
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="2" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>37</v>
@@ -2547,35 +2517,35 @@
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>38</v>
@@ -2585,16 +2555,16 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>37</v>
@@ -2604,16 +2574,16 @@
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>38</v>
@@ -2623,12 +2593,12 @@
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="23" t="s">
@@ -2642,12 +2612,12 @@
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="24" t="s">
@@ -2658,19 +2628,19 @@
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
-      <c r="H19" s="2" t="s">
-        <v>50</v>
+      <c r="H19" t="s">
+        <v>82</v>
       </c>
       <c r="I19" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>37</v>
@@ -2682,12 +2652,12 @@
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>38</v>
@@ -2699,16 +2669,16 @@
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>37</v>
@@ -2718,20 +2688,20 @@
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>37</v>
@@ -2739,20 +2709,20 @@
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>37</v>
@@ -2760,20 +2730,20 @@
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A25" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>38</v>
@@ -2781,18 +2751,18 @@
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A26" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>37</v>
@@ -2800,18 +2770,18 @@
       <c r="H26" s="2"/>
       <c r="I26" s="7"/>
     </row>
-    <row r="27" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A27" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D27" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>41</v>
@@ -2823,18 +2793,18 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A28" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D28" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>41</v>
@@ -2846,15 +2816,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A29" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>37</v>
@@ -2862,18 +2832,18 @@
       <c r="H29" s="2"/>
       <c r="I29" s="7"/>
     </row>
-    <row r="30" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A30" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F30" s="22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>37</v>
@@ -2881,37 +2851,37 @@
       <c r="H30" s="2"/>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A31" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A32" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>38</v>
@@ -2919,18 +2889,18 @@
       <c r="H32" s="2"/>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A33" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F33" s="25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>37</v>
@@ -2938,18 +2908,18 @@
       <c r="H33" s="2"/>
       <c r="I33" s="7"/>
     </row>
-    <row r="34" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A34" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>41</v>
@@ -2961,18 +2931,18 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A35" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>37</v>
@@ -2980,18 +2950,18 @@
       <c r="H35" s="2"/>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A36" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>38</v>
@@ -2999,37 +2969,37 @@
       <c r="H36" s="2"/>
       <c r="I36" s="7"/>
     </row>
-    <row r="37" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A37" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="7"/>
     </row>
-    <row r="38" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A38" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F38" s="26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>37</v>
@@ -3037,18 +3007,18 @@
       <c r="H38" s="2"/>
       <c r="I38" s="7"/>
     </row>
-    <row r="39" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A39" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>40</v>
@@ -3056,12 +3026,12 @@
       <c r="H39" s="2"/>
       <c r="I39" s="7"/>
     </row>
-    <row r="40" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A40" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D40" s="22" t="s">
         <v>44</v>
@@ -3072,12 +3042,12 @@
       <c r="H40" s="2"/>
       <c r="I40" s="7"/>
     </row>
-    <row r="41" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A41" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>44</v>
@@ -3086,18 +3056,18 @@
         <v>45</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="I41" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A42" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>37</v>
@@ -3105,12 +3075,12 @@
       <c r="H42" s="2"/>
       <c r="I42" s="7"/>
     </row>
-    <row r="43" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A43" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>38</v>
@@ -3118,12 +3088,12 @@
       <c r="H43" s="2"/>
       <c r="I43" s="7"/>
     </row>
-    <row r="44" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A44" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>37</v>
@@ -3131,12 +3101,12 @@
       <c r="H44" s="2"/>
       <c r="I44" s="7"/>
     </row>
-    <row r="45" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A45" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>38</v>
@@ -3144,12 +3114,12 @@
       <c r="H45" s="2"/>
       <c r="I45" s="7"/>
     </row>
-    <row r="46" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A46" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>37</v>
@@ -3157,59 +3127,59 @@
       <c r="H46" s="2"/>
       <c r="I46" s="7"/>
     </row>
-    <row r="47" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A47" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>45</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="I47" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A48" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="7"/>
     </row>
-    <row r="49" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A49" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H49" s="9" t="s">
-        <v>75</v>
+      <c r="H49" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="I49" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A50" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D50" s="22" t="s">
         <v>44</v>
@@ -3220,35 +3190,35 @@
       <c r="H50" s="2"/>
       <c r="I50" s="7"/>
     </row>
-    <row r="51" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A51" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>45</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="I51" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A52" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B52" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>37</v>
@@ -3256,18 +3226,18 @@
       <c r="H52" s="2"/>
       <c r="I52" s="7"/>
     </row>
-    <row r="53" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A53" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B53" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F53" s="26" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>37</v>
@@ -3275,18 +3245,18 @@
       <c r="H53" s="2"/>
       <c r="I53" s="7"/>
     </row>
-    <row r="54" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A54" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B54" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>38</v>
@@ -3294,18 +3264,18 @@
       <c r="H54" s="2"/>
       <c r="I54" s="7"/>
     </row>
-    <row r="55" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A55" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>37</v>
@@ -3313,18 +3283,18 @@
       <c r="H55" s="2"/>
       <c r="I55" s="7"/>
     </row>
-    <row r="56" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A56" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F56" s="22" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>37</v>
@@ -3332,18 +3302,18 @@
       <c r="H56" s="2"/>
       <c r="I56" s="7"/>
     </row>
-    <row r="57" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A57" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B57" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>38</v>
@@ -3351,18 +3321,18 @@
       <c r="H57" s="2"/>
       <c r="I57" s="7"/>
     </row>
-    <row r="58" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A58" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B58" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>37</v>
@@ -3370,15 +3340,15 @@
       <c r="H58" s="2"/>
       <c r="I58" s="7"/>
     </row>
-    <row r="59" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A59" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>37</v>
@@ -3386,18 +3356,18 @@
       <c r="H59" s="2"/>
       <c r="I59" s="7"/>
     </row>
-    <row r="60" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A60" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B60" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F60" s="23" t="s">
         <v>63</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F60" s="23" t="s">
-        <v>68</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>37</v>
@@ -3405,18 +3375,18 @@
       <c r="H60" s="2"/>
       <c r="I60" s="7"/>
     </row>
-    <row r="61" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A61" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B61" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F61" s="24" t="s">
         <v>63</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F61" s="24" t="s">
-        <v>68</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>38</v>
@@ -3424,18 +3394,18 @@
       <c r="H61" s="2"/>
       <c r="I61" s="7"/>
     </row>
-    <row r="62" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A62" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B62" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F62" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>37</v>
@@ -3443,18 +3413,18 @@
       <c r="H62" s="2"/>
       <c r="I62" s="7"/>
     </row>
-    <row r="63" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A63" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F63" s="26" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G63" s="3" t="s">
         <v>37</v>
@@ -3462,18 +3432,18 @@
       <c r="H63" s="2"/>
       <c r="I63" s="7"/>
     </row>
-    <row r="64" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A64" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>38</v>
@@ -3481,18 +3451,18 @@
       <c r="H64" s="2"/>
       <c r="I64" s="7"/>
     </row>
-    <row r="65" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A65" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>37</v>
@@ -3500,15 +3470,15 @@
       <c r="H65" s="2"/>
       <c r="I65" s="7"/>
     </row>
-    <row r="66" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A66" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>37</v>
@@ -3516,12 +3486,12 @@
       <c r="H66" s="2"/>
       <c r="I66" s="7"/>
     </row>
-    <row r="67" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A67" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B67" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>44</v>
@@ -3530,40 +3500,40 @@
         <v>45</v>
       </c>
       <c r="H67" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I67" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A68" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="I67" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B68" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A69" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B69" s="22" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H69" s="2"/>
       <c r="I69" s="7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' of https://github.com/AulaPlanetaColombia/CienciasSociales"
This reverts commit 08276200c400636da54b8f7263d35df29dee813c, reversing
changes made to bc636f9fd7637b0b5cfc559c92034e991d877b49.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion01/EsqueletoGuion_CS_07_01_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion01/EsqueletoGuion_CS_07_01_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\CienciasSociales\fuentes\contenidos\grado07\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MCMarquez\Desktop\Versiones\CienciasSociales\fuentes\contenidos\grado07\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3408" yWindow="226" windowWidth="22007" windowHeight="13186" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="3405" yWindow="225" windowWidth="22005" windowHeight="13185" tabRatio="729" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="93">
   <si>
     <t>FICHA</t>
   </si>
@@ -171,6 +171,9 @@
     <t>Practica</t>
   </si>
   <si>
+    <t>Refuerza tu aprendizaje: la caída del Imperio Romano de Occidente</t>
+  </si>
+  <si>
     <t>El Imperio Bizantino</t>
   </si>
   <si>
@@ -180,6 +183,9 @@
     <t>El Cisma de Oriente</t>
   </si>
   <si>
+    <t>Refuerza tu aprendizaje: el Imperio Bizantino</t>
+  </si>
+  <si>
     <t>El Imperio Islámico</t>
   </si>
   <si>
@@ -204,9 +210,18 @@
     <t>El Califato abasí o Califato de Bagdad</t>
   </si>
   <si>
+    <t>Refuerza tu aprendizaje: la expansión islámica</t>
+  </si>
+  <si>
     <t>El Imperio Carolingio</t>
   </si>
   <si>
+    <t>Comprende qué fue el Imperio Carolingio</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: el Imperio Carolingio</t>
+  </si>
+  <si>
     <t>El mundo afroasiático durante la Edad Media</t>
   </si>
   <si>
@@ -243,7 +258,13 @@
     <t>Evaluación</t>
   </si>
   <si>
+    <t>Nuevos reinos</t>
+  </si>
+  <si>
     <t>Comprender cómo el fin de una época (el Imperio Romano) es el comienzo de otra nueva con otros protagonistas y circunstancias (Imperio Bizantino, mundo musulmán, Imperio de Carlomagno).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refuerza importancia histórica de los imperios afroasiáticos en el medioevo europeo tu aprendizaje: </t>
   </si>
   <si>
     <t>Mapa conceptual</t>
@@ -282,6 +303,9 @@
     </r>
   </si>
   <si>
+    <t>Textoo</t>
+  </si>
+  <si>
     <t>El Califato Ortodoxo</t>
   </si>
   <si>
@@ -292,6 +316,12 @@
   </si>
   <si>
     <t>Conoce el Imperio bizantino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refuerza tu aprendizaje: Importancia histórica de los imperios afroasiáticos </t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Conoce el Imperio Bizantino</t>
   </si>
 </sst>
 </file>
@@ -1647,13 +1677,13 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.3984375" customWidth="1"/>
-    <col min="2" max="2" width="104.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="104.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>8</v>
       </c>
@@ -1661,7 +1691,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
@@ -1669,23 +1699,23 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="28.65" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>1</v>
       </c>
@@ -1693,7 +1723,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>12</v>
       </c>
@@ -1716,26 +1746,26 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.86328125" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.86328125" style="2"/>
-    <col min="2" max="2" width="9.265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="2"/>
+    <col min="2" max="2" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.86328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.86328125" style="2"/>
-    <col min="9" max="10" width="15.1328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.86328125" style="2"/>
+    <col min="4" max="4" width="51.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="2"/>
+    <col min="9" max="10" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -1755,7 +1785,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -1775,7 +1805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -1795,27 +1825,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1835,7 +1865,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1855,7 +1885,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -1875,7 +1905,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1886,7 +1916,7 @@
         <v>28</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>30</v>
@@ -1895,7 +1925,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -1915,27 +1945,27 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="F10" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1969,18 +1999,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.86328125" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.1328125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.73046875" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.86328125" style="2"/>
+    <col min="1" max="1" width="66.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>3</v>
       </c>
@@ -1991,40 +2021,40 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="17" customFormat="1" ht="28.65" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C2" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C3" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C4" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2049,19 +2079,19 @@
   </sheetPr>
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.73046875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>5</v>
       </c>
@@ -2072,7 +2102,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2083,7 +2113,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="28.65" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2094,18 +2124,18 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>82</v>
+      <c r="B4" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2116,7 +2146,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2127,7 +2157,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2138,84 +2168,84 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>73</v>
+      <c r="B8" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>76</v>
+      <c r="B10" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="28.65" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27" s="5"/>
     </row>
   </sheetData>
@@ -2236,25 +2266,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="61" zoomScaleNormal="61" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="61" zoomScaleNormal="61" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="H51" sqref="H51"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.265625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="46.1328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="17.86328125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="64.1328125" customWidth="1"/>
-    <col min="9" max="9" width="17.3984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="46.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="17.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="64.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>6</v>
       </c>
@@ -2283,7 +2313,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>19</v>
       </c>
@@ -2300,7 +2330,7 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>19</v>
       </c>
@@ -2317,7 +2347,7 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>19</v>
       </c>
@@ -2335,7 +2365,7 @@
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
         <v>19</v>
       </c>
@@ -2353,7 +2383,7 @@
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
         <v>19</v>
       </c>
@@ -2376,7 +2406,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>19</v>
       </c>
@@ -2387,7 +2417,7 @@
         <v>38</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>37</v>
@@ -2397,7 +2427,7 @@
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
         <v>19</v>
       </c>
@@ -2406,7 +2436,7 @@
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="23" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="22" t="s">
@@ -2418,7 +2448,7 @@
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
         <v>19</v>
       </c>
@@ -2427,7 +2457,7 @@
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="23" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="22" t="s">
@@ -2439,7 +2469,7 @@
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
         <v>19</v>
       </c>
@@ -2448,7 +2478,7 @@
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="23" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="22" t="s">
@@ -2460,7 +2490,7 @@
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
         <v>19</v>
       </c>
@@ -2478,7 +2508,7 @@
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
         <v>19</v>
       </c>
@@ -2494,18 +2524,18 @@
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="2" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>37</v>
@@ -2517,35 +2547,35 @@
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>38</v>
@@ -2555,16 +2585,16 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>37</v>
@@ -2574,16 +2604,16 @@
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>38</v>
@@ -2593,12 +2623,12 @@
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="23" t="s">
@@ -2612,12 +2642,12 @@
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="24" t="s">
@@ -2628,19 +2658,19 @@
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
-      <c r="H19" t="s">
-        <v>82</v>
+      <c r="H19" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="I19" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>37</v>
@@ -2652,12 +2682,12 @@
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>38</v>
@@ -2669,16 +2699,16 @@
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="22" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>37</v>
@@ -2688,20 +2718,20 @@
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>37</v>
@@ -2709,20 +2739,20 @@
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="22" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="24" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>37</v>
@@ -2730,20 +2760,20 @@
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>38</v>
@@ -2751,18 +2781,18 @@
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>37</v>
@@ -2770,18 +2800,18 @@
       <c r="H26" s="2"/>
       <c r="I26" s="7"/>
     </row>
-    <row r="27" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>41</v>
@@ -2793,18 +2823,18 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>41</v>
@@ -2816,15 +2846,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>37</v>
@@ -2832,18 +2862,18 @@
       <c r="H29" s="2"/>
       <c r="I29" s="7"/>
     </row>
-    <row r="30" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="F30" s="22" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>37</v>
@@ -2851,37 +2881,37 @@
       <c r="H30" s="2"/>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>38</v>
@@ -2889,18 +2919,18 @@
       <c r="H32" s="2"/>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="1:9" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="F33" s="25" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>37</v>
@@ -2908,18 +2938,18 @@
       <c r="H33" s="2"/>
       <c r="I33" s="7"/>
     </row>
-    <row r="34" spans="1:9" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>41</v>
@@ -2931,18 +2961,18 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>37</v>
@@ -2950,18 +2980,18 @@
       <c r="H35" s="2"/>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="1:9" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>38</v>
@@ -2969,37 +2999,37 @@
       <c r="H36" s="2"/>
       <c r="I36" s="7"/>
     </row>
-    <row r="37" spans="1:9" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="7"/>
     </row>
-    <row r="38" spans="1:9" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="F38" s="26" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>37</v>
@@ -3007,18 +3037,18 @@
       <c r="H38" s="2"/>
       <c r="I38" s="7"/>
     </row>
-    <row r="39" spans="1:9" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>40</v>
@@ -3026,12 +3056,12 @@
       <c r="H39" s="2"/>
       <c r="I39" s="7"/>
     </row>
-    <row r="40" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D40" s="22" t="s">
         <v>44</v>
@@ -3042,12 +3072,12 @@
       <c r="H40" s="2"/>
       <c r="I40" s="7"/>
     </row>
-    <row r="41" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>44</v>
@@ -3056,18 +3086,18 @@
         <v>45</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="I41" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>37</v>
@@ -3075,12 +3105,12 @@
       <c r="H42" s="2"/>
       <c r="I42" s="7"/>
     </row>
-    <row r="43" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>38</v>
@@ -3088,12 +3118,12 @@
       <c r="H43" s="2"/>
       <c r="I43" s="7"/>
     </row>
-    <row r="44" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>37</v>
@@ -3101,12 +3131,12 @@
       <c r="H44" s="2"/>
       <c r="I44" s="7"/>
     </row>
-    <row r="45" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>38</v>
@@ -3114,12 +3144,12 @@
       <c r="H45" s="2"/>
       <c r="I45" s="7"/>
     </row>
-    <row r="46" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>37</v>
@@ -3127,59 +3157,59 @@
       <c r="H46" s="2"/>
       <c r="I46" s="7"/>
     </row>
-    <row r="47" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>45</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="I47" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="7"/>
     </row>
-    <row r="49" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H49" s="2" t="s">
-        <v>76</v>
+      <c r="H49" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="I49" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D50" s="22" t="s">
         <v>44</v>
@@ -3190,35 +3220,35 @@
       <c r="H50" s="2"/>
       <c r="I50" s="7"/>
     </row>
-    <row r="51" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>45</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="I51" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B52" s="22" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>37</v>
@@ -3226,18 +3256,18 @@
       <c r="H52" s="2"/>
       <c r="I52" s="7"/>
     </row>
-    <row r="53" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B53" s="22" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F53" s="26" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>37</v>
@@ -3245,18 +3275,18 @@
       <c r="H53" s="2"/>
       <c r="I53" s="7"/>
     </row>
-    <row r="54" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B54" s="22" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>38</v>
@@ -3264,18 +3294,18 @@
       <c r="H54" s="2"/>
       <c r="I54" s="7"/>
     </row>
-    <row r="55" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>37</v>
@@ -3283,18 +3313,18 @@
       <c r="H55" s="2"/>
       <c r="I55" s="7"/>
     </row>
-    <row r="56" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F56" s="22" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>37</v>
@@ -3302,18 +3332,18 @@
       <c r="H56" s="2"/>
       <c r="I56" s="7"/>
     </row>
-    <row r="57" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B57" s="22" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>38</v>
@@ -3321,18 +3351,18 @@
       <c r="H57" s="2"/>
       <c r="I57" s="7"/>
     </row>
-    <row r="58" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B58" s="22" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>37</v>
@@ -3340,15 +3370,15 @@
       <c r="H58" s="2"/>
       <c r="I58" s="7"/>
     </row>
-    <row r="59" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>37</v>
@@ -3356,18 +3386,18 @@
       <c r="H59" s="2"/>
       <c r="I59" s="7"/>
     </row>
-    <row r="60" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B60" s="22" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F60" s="23" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>37</v>
@@ -3375,18 +3405,18 @@
       <c r="H60" s="2"/>
       <c r="I60" s="7"/>
     </row>
-    <row r="61" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F61" s="24" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>38</v>
@@ -3394,18 +3424,18 @@
       <c r="H61" s="2"/>
       <c r="I61" s="7"/>
     </row>
-    <row r="62" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>37</v>
@@ -3413,18 +3443,18 @@
       <c r="H62" s="2"/>
       <c r="I62" s="7"/>
     </row>
-    <row r="63" spans="1:9" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F63" s="26" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="G63" s="3" t="s">
         <v>37</v>
@@ -3432,18 +3462,18 @@
       <c r="H63" s="2"/>
       <c r="I63" s="7"/>
     </row>
-    <row r="64" spans="1:9" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>38</v>
@@ -3451,18 +3481,18 @@
       <c r="H64" s="2"/>
       <c r="I64" s="7"/>
     </row>
-    <row r="65" spans="1:9" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>37</v>
@@ -3470,15 +3500,15 @@
       <c r="H65" s="2"/>
       <c r="I65" s="7"/>
     </row>
-    <row r="66" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>37</v>
@@ -3486,12 +3516,12 @@
       <c r="H66" s="2"/>
       <c r="I66" s="7"/>
     </row>
-    <row r="67" spans="1:9" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B67" s="22" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>44</v>
@@ -3500,40 +3530,40 @@
         <v>45</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="I67" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B68" s="22" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B69" s="22" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="H69" s="2"/>
       <c r="I69" s="7" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>